<commit_message>
Updates details in spreadsheet
</commit_message>
<xml_diff>
--- a/BiophotonicsMeetingMaster.xlsx
+++ b/BiophotonicsMeetingMaster.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Matt Goodwin\Documents\Github\BiophotonicsEmailBot\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34AC688A-8C9A-464C-833A-ED12E3EA1B09}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{266B917F-939A-4F31-AF2A-B56C2867220F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1114,7 +1114,7 @@
   <dimension ref="A1:H40"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="H34" sqref="H34"/>
+      <selection activeCell="K41" sqref="K41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>